<commit_message>
add table view laporan lipa 6
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_6.xlsx
+++ b/hasil/2023_01_lipa_6.xlsx
@@ -89,7 +89,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 02 Agustus 2023</t>
+    <t>Ternate , 04 September 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -1125,13 +1125,13 @@
         <v>0</v>
       </c>
       <c r="E9" s="15">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="15">
         <v>6</v>
       </c>
       <c r="G9" s="15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="15">
         <v>6</v>
@@ -1143,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L9" s="15">
         <v>4</v>
@@ -1176,13 +1176,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="15">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F10" s="15">
         <v>0</v>
       </c>
       <c r="G10" s="15">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H10" s="15">
         <v>0</v>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="15">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L10" s="15">
         <v>0</v>
@@ -1227,13 +1227,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="15">
         <v>4</v>
       </c>
       <c r="G11" s="15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11" s="15">
         <v>4</v>
@@ -1245,7 +1245,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="15">
         <v>1</v>
@@ -1277,13 +1277,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="15">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="15">
         <v>3</v>
       </c>
       <c r="G12" s="15">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="15">
         <v>3</v>
@@ -1295,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L12" s="15">
         <v>0</v>
@@ -1377,13 +1377,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="15">
         <v>1</v>
       </c>
       <c r="G14" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H14" s="15">
         <v>1</v>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L14" s="15">
         <v>1</v>

</xml_diff>